<commit_message>
Assigned some footprints, finished BOM
</commit_message>
<xml_diff>
--- a/Hardware/Processor_Periph/Processor.xlsx
+++ b/Hardware/Processor_Periph/Processor.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="211">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -226,7 +226,16 @@
     <t xml:space="preserve">Micro_SD_Card</t>
   </si>
   <si>
-    <t xml:space="preserve">J1 J2 J6 JP1</t>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x4 Male Header (Right Angle)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2 J6 JP1</t>
   </si>
   <si>
     <t xml:space="preserve">I2C</t>
@@ -980,10 +989,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1381,11 +1390,11 @@
         <v>68</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="n">
         <f aca="false">B17*3</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>69</v>
@@ -1393,97 +1402,91 @@
       <c r="E17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">B18*3</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="H18" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>610112249121</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">B19*3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="0" t="n">
+        <v>610112249121</v>
+      </c>
+      <c r="G19" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="H19" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">B20*3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>86</v>
+      <c r="H20" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -1493,48 +1496,45 @@
         <v>3</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">B22*3</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>4</v>
@@ -1544,45 +1544,48 @@
         <v>12</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">B24*3</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D24" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="G24" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
@@ -1592,283 +1595,283 @@
         <v>3</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">B26*3</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">B27*3</f>
+        <v>12</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="F27" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">B28*3</f>
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="G28" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">B29*3</f>
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">B30*3</f>
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">B31*3</f>
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">B32*3</f>
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">B33*3</f>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">B34*3</f>
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="G34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">B35*3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D35" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>144</v>
-      </c>
       <c r="G35" s="5" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">B36*3</f>
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E36" s="7" t="n">
-        <v>5019</v>
-      </c>
-      <c r="F36" s="5" t="n">
-        <v>5019</v>
-      </c>
-      <c r="G36" s="8" t="s">
         <v>150</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,28 +1879,28 @@
         <v>151</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">B37*3</f>
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="7" t="n">
+        <v>5019</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -1907,15 +1910,15 @@
         <v>3</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="G38" s="0" t="s">
+      <c r="G38" s="5" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1933,22 +1936,19 @@
       <c r="D39" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="G39" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -1958,24 +1958,24 @@
         <v>3</v>
       </c>
       <c r="D40" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="H40" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -1985,21 +1985,24 @@
         <v>3</v>
       </c>
       <c r="D41" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="G41" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F41" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>174</v>
+      <c r="H41" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -2009,21 +2012,21 @@
         <v>3</v>
       </c>
       <c r="D42" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="G42" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -2033,21 +2036,21 @@
         <v>3</v>
       </c>
       <c r="D43" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="G43" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
@@ -2057,21 +2060,21 @@
         <v>3</v>
       </c>
       <c r="D44" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="0" t="s">
+      <c r="G44" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
@@ -2081,75 +2084,72 @@
         <v>3</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="G45" s="0" t="s">
         <v>191</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="0" t="n">
         <f aca="false">B46*3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D46" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="G46" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" s="0" t="n">
         <f aca="false">B47*3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D47" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F47" s="5" t="s">
+      <c r="H47" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -2159,16 +2159,43 @@
         <v>3</v>
       </c>
       <c r="D48" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="G48" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <f aca="false">B49*3</f>
+        <v>3</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>207</v>
+      <c r="F49" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>